<commit_message>
added megas and AI update
added every mega bar beak
made so the AI understands field/weather setting abilities on megaing
</commit_message>
<xml_diff>
--- a/calcStats_calcHP.xlsx
+++ b/calcStats_calcHP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\project-untamed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BF5730-BCCB-45AC-927F-BD81FC222790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B99C7C-E4B1-4D88-931B-280941FE51A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FEE3E248-0CFB-47B3-A821-C02253D73434}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t>hp</t>
   </si>
@@ -61,14 +61,18 @@
   </si>
   <si>
     <t>Burbrawl</t>
+  </si>
+  <si>
+    <t>stat mult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -99,13 +103,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,18 +425,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA952E08-3A74-4E58-9935-D972A9C035A8}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="J8" sqref="J8:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="7" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -442,7 +451,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -464,8 +473,29 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>76</v>
       </c>
@@ -488,37 +518,86 @@
         <f>SUM(A3:F3)</f>
         <v>569</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>80</v>
+      </c>
+      <c r="M3">
+        <v>70</v>
+      </c>
+      <c r="N3">
+        <v>110</v>
+      </c>
+      <c r="O3">
+        <f>SUM(I3:N3)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>"max " &amp; A$2</f>
+        <f t="shared" ref="A4:F4" si="0">"max " &amp; A$2</f>
         <v>max hp</v>
       </c>
       <c r="B4" t="str">
-        <f>"max " &amp; B$2</f>
+        <f t="shared" si="0"/>
         <v>max atk</v>
       </c>
       <c r="C4" t="str">
-        <f>"max " &amp; C$2</f>
+        <f t="shared" si="0"/>
         <v>max def</v>
       </c>
       <c r="D4" t="str">
-        <f>"max " &amp; D$2</f>
+        <f t="shared" si="0"/>
         <v>max speed</v>
       </c>
       <c r="E4" t="str">
-        <f>"max " &amp; E$2</f>
+        <f t="shared" si="0"/>
         <v>max spatk</v>
       </c>
       <c r="F4" t="str">
-        <f>"max " &amp; F$2</f>
+        <f t="shared" si="0"/>
         <v>max spdef</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" t="str">
+        <f>"mega " &amp; I$2</f>
+        <v>mega hp</v>
+      </c>
+      <c r="J4" t="str">
+        <f>"mega " &amp; J$2</f>
+        <v>mega atk</v>
+      </c>
+      <c r="K4" t="str">
+        <f>"mega " &amp; K$2</f>
+        <v>mega def</v>
+      </c>
+      <c r="L4" t="str">
+        <f>"mega " &amp; L$2</f>
+        <v>mega speed</v>
+      </c>
+      <c r="M4" t="str">
+        <f>"mega " &amp; M$2</f>
+        <v>mega spatk</v>
+      </c>
+      <c r="N4" t="str">
+        <f>"mega " &amp; N$2</f>
+        <v>mega spdef</v>
+      </c>
+      <c r="O4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>(((((A3 * 2)) * 100 / 100) + 100 + 10))</f>
         <v>262</v>
@@ -528,26 +607,77 @@
         <v>276</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:F5" si="0">ROUNDDOWN(((((((C3*2))*100/100)+5)*110/100)),0)</f>
+        <f t="shared" ref="C5:F5" si="1">ROUNDDOWN(((((((C3*2))*100/100)+5)*110/100)),0)</f>
         <v>139</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>273</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>254</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>50</v>
+      </c>
+      <c r="J5">
+        <v>72</v>
+      </c>
+      <c r="K5">
+        <v>55</v>
+      </c>
+      <c r="L5">
+        <v>103</v>
+      </c>
+      <c r="M5">
+        <v>110</v>
+      </c>
+      <c r="N5">
+        <v>130</v>
+      </c>
+      <c r="O5">
+        <f>SUM(I5:N5)</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I6" t="str">
+        <f t="shared" ref="I6:N6" si="2">"max " &amp; I$2</f>
+        <v>max hp</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="2"/>
+        <v>max atk</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="2"/>
+        <v>max def</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>max speed</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="2"/>
+        <v>max spatk</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="2"/>
+        <v>max spdef</v>
+      </c>
+      <c r="O6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -557,8 +687,35 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f>(((((I5 * 2)) * 100 / 100) + 100 + 10))</f>
+        <v>210</v>
+      </c>
+      <c r="J7" s="2">
+        <f>ROUNDDOWN(((((((J5*2))*100/100)+5)*110/100)),0)</f>
+        <v>163</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" ref="K7:N7" si="3">ROUNDDOWN(((((((K5*2))*100/100)+5)*110/100)),0)</f>
+        <v>126</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="3"/>
+        <v>247</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="3"/>
+        <v>291</v>
+      </c>
+      <c r="O7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -580,8 +737,35 @@
       <c r="G8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" ref="J8:N8" si="4">J5/J3</f>
+        <v>1.2</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="4"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L8" s="4">
+        <f>L5/L3</f>
+        <v>1.2875000000000001</v>
+      </c>
+      <c r="M8" s="4">
+        <f t="shared" si="4"/>
+        <v>1.5714285714285714</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="4"/>
+        <v>1.1818181818181819</v>
+      </c>
+      <c r="O8">
+        <f>O5-O3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>77</v>
       </c>
@@ -605,36 +789,36 @@
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>"max " &amp; A$2</f>
+        <f t="shared" ref="A10:F10" si="5">"max " &amp; A$2</f>
         <v>max hp</v>
       </c>
       <c r="B10" t="str">
-        <f>"max " &amp; B$2</f>
+        <f t="shared" si="5"/>
         <v>max atk</v>
       </c>
       <c r="C10" t="str">
-        <f>"max " &amp; C$2</f>
+        <f t="shared" si="5"/>
         <v>max def</v>
       </c>
       <c r="D10" t="str">
-        <f>"max " &amp; D$2</f>
+        <f t="shared" si="5"/>
         <v>max speed</v>
       </c>
       <c r="E10" t="str">
-        <f>"max " &amp; E$2</f>
+        <f t="shared" si="5"/>
         <v>max spatk</v>
       </c>
       <c r="F10" t="str">
-        <f>"max " &amp; F$2</f>
+        <f t="shared" si="5"/>
         <v>max spdef</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>(((((A9 * 2)) * 100 / 100) + 100 + 10))</f>
         <v>264</v>
@@ -644,29 +828,29 @@
         <v>227</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" ref="C11:F11" si="1">ROUNDDOWN(((((((C9*2))*100/100)+5)*110/100)),0)</f>
+        <f t="shared" ref="C11:F11" si="6">ROUNDDOWN(((((((C9*2))*100/100)+5)*110/100)),0)</f>
         <v>236</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>86</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>199</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -677,7 +861,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -700,7 +884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>40</v>
       </c>
@@ -724,29 +908,29 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>"max " &amp; A$2</f>
+        <f t="shared" ref="A16:F16" si="7">"max " &amp; A$2</f>
         <v>max hp</v>
       </c>
       <c r="B16" t="str">
-        <f>"max " &amp; B$2</f>
+        <f t="shared" si="7"/>
         <v>max atk</v>
       </c>
       <c r="C16" t="str">
-        <f>"max " &amp; C$2</f>
+        <f t="shared" si="7"/>
         <v>max def</v>
       </c>
       <c r="D16" t="str">
-        <f>"max " &amp; D$2</f>
+        <f t="shared" si="7"/>
         <v>max speed</v>
       </c>
       <c r="E16" t="str">
-        <f>"max " &amp; E$2</f>
+        <f t="shared" si="7"/>
         <v>max spatk</v>
       </c>
       <c r="F16" t="str">
-        <f>"max " &amp; F$2</f>
+        <f t="shared" si="7"/>
         <v>max spdef</v>
       </c>
       <c r="G16" t="s">
@@ -763,19 +947,19 @@
         <v>159</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" ref="C17:F17" si="2">ROUNDDOWN(((((((C15*2))*100/100)+5)*110/100)),0)</f>
+        <f t="shared" ref="C17:F17" si="8">ROUNDDOWN(((((((C15*2))*100/100)+5)*110/100)),0)</f>
         <v>60</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>159</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>104</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>71</v>
       </c>
       <c r="G17" t="s">

</xml_diff>

<commit_message>
both mega beakraft and AI edits
</commit_message>
<xml_diff>
--- a/calcStats_calcHP.xlsx
+++ b/calcStats_calcHP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\project-untamed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B99C7C-E4B1-4D88-931B-280941FE51A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A69B21-5C38-4BE7-9097-A44253F6A66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FEE3E248-0CFB-47B3-A821-C02253D73434}"/>
   </bookViews>
@@ -107,10 +107,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,15 +441,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -519,26 +519,26 @@
         <v>569</v>
       </c>
       <c r="I3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="J3">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="K3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="L3">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="M3">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="N3">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="O3">
         <f>SUM(I3:N3)</f>
-        <v>420</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -570,27 +570,27 @@
         <v>7</v>
       </c>
       <c r="I4" t="str">
-        <f>"mega " &amp; I$2</f>
+        <f t="shared" ref="I4:N4" si="1">"mega " &amp; I$2</f>
         <v>mega hp</v>
       </c>
       <c r="J4" t="str">
-        <f>"mega " &amp; J$2</f>
+        <f t="shared" si="1"/>
         <v>mega atk</v>
       </c>
       <c r="K4" t="str">
-        <f>"mega " &amp; K$2</f>
+        <f t="shared" si="1"/>
         <v>mega def</v>
       </c>
       <c r="L4" t="str">
-        <f>"mega " &amp; L$2</f>
+        <f t="shared" si="1"/>
         <v>mega speed</v>
       </c>
       <c r="M4" t="str">
-        <f>"mega " &amp; M$2</f>
+        <f t="shared" si="1"/>
         <v>mega spatk</v>
       </c>
       <c r="N4" t="str">
-        <f>"mega " &amp; N$2</f>
+        <f t="shared" si="1"/>
         <v>mega spdef</v>
       </c>
       <c r="O4" t="s">
@@ -607,70 +607,70 @@
         <v>276</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:F5" si="1">ROUNDDOWN(((((((C3*2))*100/100)+5)*110/100)),0)</f>
+        <f t="shared" ref="C5:F5" si="2">ROUNDDOWN(((((((C3*2))*100/100)+5)*110/100)),0)</f>
         <v>139</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>273</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>254</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>168</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
       <c r="I5">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="J5">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="K5">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="L5">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="M5">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="N5">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="O5">
         <f>SUM(I5:N5)</f>
-        <v>520</v>
+        <v>585</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I6" t="str">
-        <f t="shared" ref="I6:N6" si="2">"max " &amp; I$2</f>
+        <f t="shared" ref="I6:N6" si="3">"max " &amp; I$2</f>
         <v>max hp</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>max atk</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>max def</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>max speed</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>max spatk</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>max spdef</v>
       </c>
       <c r="O6" t="s">
@@ -678,38 +678,38 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="I7">
         <f>(((((I5 * 2)) * 100 / 100) + 100 + 10))</f>
-        <v>210</v>
+        <v>260</v>
       </c>
       <c r="J7" s="2">
         <f>ROUNDDOWN(((((((J5*2))*100/100)+5)*110/100)),0)</f>
-        <v>163</v>
+        <v>236</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" ref="K7:N7" si="3">ROUNDDOWN(((((((K5*2))*100/100)+5)*110/100)),0)</f>
-        <v>126</v>
+        <f t="shared" ref="K7:N7" si="4">ROUNDDOWN(((((((K5*2))*100/100)+5)*110/100)),0)</f>
+        <v>170</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="3"/>
-        <v>232</v>
+        <f t="shared" si="4"/>
+        <v>159</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="3"/>
-        <v>247</v>
+        <f t="shared" si="4"/>
+        <v>302</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="3"/>
-        <v>291</v>
+        <f t="shared" si="4"/>
+        <v>280</v>
       </c>
       <c r="O7" t="s">
         <v>8</v>
@@ -737,28 +737,28 @@
       <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="4">
-        <f t="shared" ref="J8:N8" si="4">J5/J3</f>
-        <v>1.2</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="4"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="J8" s="3">
+        <f t="shared" ref="J8:N8" si="5">J5/J3</f>
+        <v>1.4</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
         <f>L5/L3</f>
-        <v>1.2875000000000001</v>
-      </c>
-      <c r="M8" s="4">
-        <f t="shared" si="4"/>
-        <v>1.5714285714285714</v>
-      </c>
-      <c r="N8" s="4">
-        <f t="shared" si="4"/>
-        <v>1.1818181818181819</v>
+        <v>1.75</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="5"/>
+        <v>1.08</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="5"/>
+        <v>1.3157894736842106</v>
       </c>
       <c r="O8">
         <f>O5-O3</f>
@@ -791,27 +791,27 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" ref="A10:F10" si="5">"max " &amp; A$2</f>
+        <f t="shared" ref="A10:F10" si="6">"max " &amp; A$2</f>
         <v>max hp</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>max atk</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>max def</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>max speed</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>max spatk</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>max spdef</v>
       </c>
       <c r="G10" t="s">
@@ -828,19 +828,19 @@
         <v>227</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" ref="C11:F11" si="6">ROUNDDOWN(((((((C9*2))*100/100)+5)*110/100)),0)</f>
+        <f t="shared" ref="C11:F11" si="7">ROUNDDOWN(((((((C9*2))*100/100)+5)*110/100)),0)</f>
         <v>236</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>86</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>199</v>
       </c>
       <c r="G11" t="s">
@@ -851,15 +851,15 @@
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -910,27 +910,27 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" ref="A16:F16" si="7">"max " &amp; A$2</f>
+        <f t="shared" ref="A16:F16" si="8">"max " &amp; A$2</f>
         <v>max hp</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>max atk</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>max def</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>max speed</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>max spatk</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>max spdef</v>
       </c>
       <c r="G16" t="s">
@@ -947,19 +947,19 @@
         <v>159</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" ref="C17:F17" si="8">ROUNDDOWN(((((((C15*2))*100/100)+5)*110/100)),0)</f>
+        <f t="shared" ref="C17:F17" si="9">ROUNDDOWN(((((((C15*2))*100/100)+5)*110/100)),0)</f>
         <v>60</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>159</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>71</v>
       </c>
       <c r="G17" t="s">

</xml_diff>

<commit_message>
holy shit thats some good compression right fucking there
</commit_message>
<xml_diff>
--- a/calcStats_calcHP.xlsx
+++ b/calcStats_calcHP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\project-untamed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE52DB6A-7C2A-48D4-8D63-69E9A46E3B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32634980-10EB-411E-8F4C-C233502433A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FEE3E248-0CFB-47B3-A821-C02253D73434}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,26 +519,26 @@
         <v>569</v>
       </c>
       <c r="I3">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J3">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="K3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L3">
         <v>85</v>
       </c>
       <c r="M3">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="N3">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O3">
         <f>SUM(I3:N3)</f>
-        <v>390</v>
+        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -626,26 +626,26 @@
         <v>8</v>
       </c>
       <c r="I5">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="J5">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="K5">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="L5">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M5">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="N5">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="O5">
         <f>SUM(I5:N5)</f>
-        <v>492</v>
+        <v>590</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -689,27 +689,27 @@
       <c r="G7" s="4"/>
       <c r="I7">
         <f>(((((I5 * 2)) * 100 / 100) + 100 + 10))</f>
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J7" s="2">
         <f>ROUNDDOWN(((((((J5*2))*100/100)+5)*110/100)),0)</f>
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ref="K7:N7" si="4">ROUNDDOWN(((((((K5*2))*100/100)+5)*110/100)),0)</f>
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="4"/>
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="4"/>
-        <v>86</v>
+        <v>302</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="4"/>
-        <v>262</v>
+        <v>324</v>
       </c>
       <c r="O7" t="s">
         <v>8</v>
@@ -742,27 +742,27 @@
       </c>
       <c r="J8" s="3">
         <f t="shared" ref="J8:N8" si="5">J5/J3</f>
-        <v>1.9454545454545455</v>
+        <v>1.1176470588235294</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" si="5"/>
-        <v>1.54</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="L8" s="3">
         <f>L5/L3</f>
-        <v>1.0235294117647058</v>
+        <v>1</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="5"/>
-        <v>1.0571428571428572</v>
+        <v>1.4210526315789473</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="5"/>
-        <v>1.0636363636363637</v>
+        <v>1.3809523809523809</v>
       </c>
       <c r="O8">
         <f>O5-O3</f>
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>